<commit_message>
1)edit excel 2)add role condition in employee index function
</commit_message>
<xml_diff>
--- a/public/storage/uploads/importAdmin.xlsx
+++ b/public/storage/uploads/importAdmin.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laragon_Projects\School-Management-System\storage\app\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC71A3B-B0E5-4D54-A613-B1880F234031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A6E160-B923-497E-8EBF-BA28137E9EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{95E1506A-7C2F-4123-91F9-6D34E5E32F71}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Department</t>
   </si>
   <si>
-    <t>TeachingStuff</t>
-  </si>
-  <si>
     <t>Worker</t>
   </si>
   <si>
@@ -67,6 +64,12 @@
   </si>
   <si>
     <t>Financial</t>
+  </si>
+  <si>
+    <t>Teaching Staff</t>
+  </si>
+  <si>
+    <t>Student Affairs</t>
   </si>
 </sst>
 </file>
@@ -427,11 +430,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF297C12-6CB5-4643-839C-9DCA9CE43ADD}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,6 +463,11 @@
       </c>
       <c r="F1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="E4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -481,7 +489,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA92392-9FE2-4B13-8145-151575AE4B50}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -491,22 +499,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>